<commit_message>
front end upgrades - backend remaining
</commit_message>
<xml_diff>
--- a/uploads/802576637_invoices.xlsx
+++ b/uploads/802576637_invoices.xlsx
@@ -498,7 +498,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>400011062938530</t>
+          <t>400010850816176</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -506,45 +506,41 @@
           <t>802576637</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>ΤΡΑΚΑΔΑΣ Α.Ε.</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>11Μ0ΤΔΑ</t>
+          <t>TΔA</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>7836</t>
+          <t>59341</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>24/09/2025</t>
+          <t>06/09/2025</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1.1</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>41,57</t>
+          <t>-20,16</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>9,98</t>
+          <t>-4,84</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>51,55</t>
+          <t>-25,00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr"/>
@@ -552,7 +548,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>400010850816176</t>
+          <t>400011062938530</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -560,41 +556,45 @@
           <t>802576637</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ΤΡΑΚΑΔΑΣ Α.Ε.</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>TΔA</t>
+          <t>11Μ0ΤΔΑ</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>59341</t>
+          <t>7836</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>06/09/2025</t>
+          <t>24/09/2025</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>1.1</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>-20,16</t>
+          <t>41,57</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>-4,84</t>
+          <t>9,98</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>-25,00</t>
+          <t>51,55</t>
         </is>
       </c>
       <c r="L3" t="inlineStr"/>

</xml_diff>

<commit_message>
save & append to excel complete
</commit_message>
<xml_diff>
--- a/uploads/802576637_invoices.xlsx
+++ b/uploads/802576637_invoices.xlsx
@@ -493,7 +493,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>400011184830173</t>
+          <t>400011185825004</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -501,15 +501,19 @@
           <t>802576637</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ΤΡΑΚΑΔΑΣ Α.Ε.</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>TΔA</t>
+          <t>8Μ0ΤΔΑ</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>60038</t>
+          <t>8961</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -525,17 +529,17 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>18,30</t>
+          <t>22,61</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>4,39</t>
+          <t>5,43</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>22,69</t>
+          <t>28,04</t>
         </is>
       </c>
     </row>

</xml_diff>